<commit_message>
Swagger configuration added and TooManySheetsException created
</commit_message>
<xml_diff>
--- a/Back-end/sheetmanager/UploadFolder/file_example_XLSX_100_1.xlsx
+++ b/Back-end/sheetmanager/UploadFolder/file_example_XLSX_100_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="113">
   <si>
     <t>First Name</t>
   </si>
@@ -171,6 +171,186 @@
   </si>
   <si>
     <t>Curren</t>
+  </si>
+  <si>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Strawn</t>
+  </si>
+  <si>
+    <t>Belinda</t>
+  </si>
+  <si>
+    <t>Partain</t>
+  </si>
+  <si>
+    <t>Holly</t>
+  </si>
+  <si>
+    <t>Eudy</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>Cuccia</t>
+  </si>
+  <si>
+    <t>Libbie</t>
+  </si>
+  <si>
+    <t>Dalby</t>
+  </si>
+  <si>
+    <t>Lester</t>
+  </si>
+  <si>
+    <t>Prothro</t>
+  </si>
+  <si>
+    <t>Marvel</t>
+  </si>
+  <si>
+    <t>Hail</t>
+  </si>
+  <si>
+    <t>Angelyn</t>
+  </si>
+  <si>
+    <t>Vong</t>
+  </si>
+  <si>
+    <t>Francesca</t>
+  </si>
+  <si>
+    <t>Beaudreau</t>
+  </si>
+  <si>
+    <t>Garth</t>
+  </si>
+  <si>
+    <t>Gangi</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>Trumbull</t>
+  </si>
+  <si>
+    <t>Veta</t>
+  </si>
+  <si>
+    <t>Muntz</t>
+  </si>
+  <si>
+    <t>Stasia</t>
+  </si>
+  <si>
+    <t>Becker</t>
+  </si>
+  <si>
+    <t>Jona</t>
+  </si>
+  <si>
+    <t>Grindle</t>
+  </si>
+  <si>
+    <t>Judie</t>
+  </si>
+  <si>
+    <t>Claywell</t>
+  </si>
+  <si>
+    <t>Dewitt</t>
+  </si>
+  <si>
+    <t>Borger</t>
+  </si>
+  <si>
+    <t>Nena</t>
+  </si>
+  <si>
+    <t>Hacker</t>
+  </si>
+  <si>
+    <t>Kelsie</t>
+  </si>
+  <si>
+    <t>Wachtel</t>
+  </si>
+  <si>
+    <t>Sau</t>
+  </si>
+  <si>
+    <t>Pfau</t>
+  </si>
+  <si>
+    <t>Shanice</t>
+  </si>
+  <si>
+    <t>Mccrystal</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Karner</t>
+  </si>
+  <si>
+    <t>Tommie</t>
+  </si>
+  <si>
+    <t>Underdahl</t>
+  </si>
+  <si>
+    <t>Dorcas</t>
+  </si>
+  <si>
+    <t>Darity</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Sanor</t>
+  </si>
+  <si>
+    <t>Willodean</t>
+  </si>
+  <si>
+    <t>Harn</t>
+  </si>
+  <si>
+    <t>Weston</t>
+  </si>
+  <si>
+    <t>Martina</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Lafollette</t>
+  </si>
+  <si>
+    <t>Felisa</t>
+  </si>
+  <si>
+    <t>Cail</t>
+  </si>
+  <si>
+    <t>Demetria</t>
+  </si>
+  <si>
+    <t>Abbey</t>
+  </si>
+  <si>
+    <t>Jeromy</t>
+  </si>
+  <si>
+    <t>Danz</t>
   </si>
 </sst>
 </file>
@@ -215,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -741,6 +921,786 @@
         <v>9654.0</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F21" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H21" t="n" s="0">
+        <v>3569.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F22" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H22" t="n" s="0">
+        <v>2564.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>52.0</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H23" t="n" s="0">
+        <v>8561.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F24" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H24" t="n" s="0">
+        <v>5489.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F25" t="n" s="0">
+        <v>42.0</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H25" t="n" s="0">
+        <v>5489.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F26" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H26" t="n" s="0">
+        <v>6574.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F27" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H27" t="n" s="0">
+        <v>5555.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H28" t="n" s="0">
+        <v>6125.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F29" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H29" t="n" s="0">
+        <v>5412.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F30" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H30" t="n" s="0">
+        <v>3256.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F31" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H31" t="n" s="0">
+        <v>3264.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F32" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H32" t="n" s="0">
+        <v>4569.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F33" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H33" t="n" s="0">
+        <v>7521.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F34" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H34" t="n" s="0">
+        <v>6458.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F35" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H35" t="n" s="0">
+        <v>7569.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F36" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H36" t="n" s="0">
+        <v>8514.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="G37" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H37" t="n" s="0">
+        <v>8563.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="G38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H38" t="n" s="0">
+        <v>8642.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H39" t="n" s="0">
+        <v>9536.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H40" t="n" s="0">
+        <v>2567.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="G41" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H41" t="n" s="0">
+        <v>2154.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F42" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G42" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H42" t="n" s="0">
+        <v>3265.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="0">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="G43" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H43" t="n" s="0">
+        <v>8765.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F44" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H44" t="n" s="0">
+        <v>3259.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n" s="0">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F45" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="G45" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H45" t="n" s="0">
+        <v>3567.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F46" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G46" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H46" t="n" s="0">
+        <v>6540.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F47" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="G47" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H47" t="n" s="0">
+        <v>2654.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n" s="0">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F48" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="G48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H48" t="n" s="0">
+        <v>6525.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n" s="0">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F49" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="G49" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="H49" t="n" s="0">
+        <v>3265.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n" s="0">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F50" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="G50" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H50" t="n" s="0">
+        <v>3265.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>